<commit_message>
solved bug in checkout test class
</commit_message>
<xml_diff>
--- a/src/loginCredentials.xlsx
+++ b/src/loginCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DepiSwTesting\finalProj\Test\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340741C1-3BE6-4DFF-BA8C-09A66DB95B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69D91F1-DF23-407C-8969-547D956A97A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,17 +502,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>